<commit_message>
actual actual final commit
</commit_message>
<xml_diff>
--- a/Sprintplanning/006 - User Story Map - sliced.xlsx
+++ b/Sprintplanning/006 - User Story Map - sliced.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SCHUB05\Documents\InfoSupport\Eindcase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SCHUB05\Documents\InfoSupport\Eindcase\Eindcase\Sprintplanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8A6BE5-CB56-42C8-9119-AD8EEC018499}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73F7E42-AA41-440A-944A-77BF3B79E668}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="411" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="411" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cursusadministatie User Stories" sheetId="3" r:id="rId1"/>
@@ -907,7 +907,9 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent6" xfId="3" builtinId="50"/>
@@ -1227,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AJ50"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,17 +1436,17 @@
       <c r="E8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="48" t="s">
         <v>29</v>
       </c>
       <c r="J8" s="4"/>
-      <c r="O8" s="17" t="s">
+      <c r="O8" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="S8" s="17" t="s">
+      <c r="S8" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="U8" s="17" t="s">
+      <c r="U8" s="48" t="s">
         <v>25</v>
       </c>
       <c r="W8"/>
@@ -1487,14 +1489,14 @@
       </c>
       <c r="B11" s="38"/>
       <c r="C11" s="39"/>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="48" t="s">
         <v>38</v>
       </c>
       <c r="J11" s="4"/>
-      <c r="S11" s="17" t="s">
+      <c r="S11" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="U11" s="17" t="s">
+      <c r="U11" s="48" t="s">
         <v>72</v>
       </c>
       <c r="W11"/>
@@ -1539,10 +1541,10 @@
       <c r="B14" s="41"/>
       <c r="C14" s="42"/>
       <c r="J14" s="4"/>
-      <c r="S14" s="17" t="s">
+      <c r="S14" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="U14" s="17" t="s">
+      <c r="U14" s="48" t="s">
         <v>36</v>
       </c>
       <c r="W14"/>
@@ -1581,7 +1583,7 @@
       </c>
       <c r="B17" s="38"/>
       <c r="C17" s="39"/>
-      <c r="I17" s="17" t="s">
+      <c r="I17" s="48" t="s">
         <v>48</v>
       </c>
       <c r="J17" s="4"/>
@@ -1621,10 +1623,10 @@
       <c r="A20" s="40"/>
       <c r="B20" s="41"/>
       <c r="C20" s="42"/>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="I20" s="48" t="s">
         <v>57</v>
       </c>
       <c r="J20" s="4"/>
@@ -1722,7 +1724,7 @@
       </c>
       <c r="B26" s="38"/>
       <c r="C26" s="39"/>
-      <c r="G26" s="17" t="s">
+      <c r="G26" s="48" t="s">
         <v>64</v>
       </c>
       <c r="I26" s="4"/>
@@ -2174,8 +2176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2549,26 +2551,26 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="48" t="s">
+    <row r="15" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="B15" s="48">
+      <c r="B15" s="25">
         <v>9</v>
       </c>
-      <c r="C15" s="48">
+      <c r="C15" s="25">
         <v>1</v>
       </c>
-      <c r="D15" s="48" t="s">
+      <c r="D15" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="48" t="s">
+      <c r="E15" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="48" t="s">
+      <c r="F15" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="H15" s="48" t="s">
+      <c r="H15" s="25" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>